<commit_message>
Added test relation data to simpel_vergelijking_template2.xlsx
</commit_message>
<xml_diff>
--- a/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template2.xlsx
+++ b/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template2.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\job_related\wegen_en_verkeer\new_python_otl_wizard\testData\simpel_vergelijkings_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\OTLMOW-GUI\demo_projects\simpel_vergelijkings_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEE3D207-4EB5-4D94-A082-318158D7157F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5D258F-BB47-4738-B60B-E7E89163621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="installatie#Verkeersbordopstell" sheetId="1" r:id="rId1"/>
     <sheet name="onderdeel#Funderingsmassief" sheetId="2" r:id="rId2"/>
     <sheet name="onderdeel#Pictogram" sheetId="3" r:id="rId3"/>
     <sheet name="onderdeel#Verkeersbordsteun" sheetId="4" r:id="rId4"/>
-    <sheet name="Keuzelijsten" sheetId="5" r:id="rId5"/>
+    <sheet name="onderdeel#Bevestiging" sheetId="6" r:id="rId5"/>
+    <sheet name="onderdeel#HoortBij" sheetId="7" r:id="rId6"/>
+    <sheet name="onderdeel#LigtOp" sheetId="8" r:id="rId7"/>
+    <sheet name="Keuzelijsten" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="240">
   <si>
     <t>typeURI</t>
   </si>
@@ -682,16 +684,87 @@
   </si>
   <si>
     <t>video-avi</t>
+  </si>
+  <si>
+    <t>bron.typeURI</t>
+  </si>
+  <si>
+    <t>bronAssetId.identificator</t>
+  </si>
+  <si>
+    <t>bronAssetId.toegekendDoor</t>
+  </si>
+  <si>
+    <t>doel.typeURI</t>
+  </si>
+  <si>
+    <t>doelAssetId.identificator</t>
+  </si>
+  <si>
+    <t>doelAssetId.toegekendDoor</t>
+  </si>
+  <si>
+    <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Bevestiging</t>
+  </si>
+  <si>
+    <t>dummy_hXI</t>
+  </si>
+  <si>
+    <t>dummy_zQp</t>
+  </si>
+  <si>
+    <t>dummy_Ej</t>
+  </si>
+  <si>
+    <t>dummy_Q</t>
+  </si>
+  <si>
+    <t>dummy_okopD</t>
+  </si>
+  <si>
+    <t>dummy_tCIvXsNGzb</t>
+  </si>
+  <si>
+    <t>dummy_bcjseEAj</t>
+  </si>
+  <si>
+    <t>dummy_dY</t>
+  </si>
+  <si>
+    <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#HoortBij</t>
+  </si>
+  <si>
+    <t>self_assigned</t>
+  </si>
+  <si>
+    <t>dummy_LxexRM</t>
+  </si>
+  <si>
+    <t>dummy_Ouee</t>
+  </si>
+  <si>
+    <t>dummy_ZT</t>
+  </si>
+  <si>
+    <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#LigtOp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -714,13 +787,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1023,14 +1099,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="19" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1148,7 +1226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1251,14 +1329,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="19" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1317,7 +1397,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -1376,7 +1456,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1467,14 +1547,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -1556,7 +1638,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1629,14 +1711,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1698,7 +1782,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -1760,7 +1844,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -1857,17 +1941,317 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8E9B60-EC96-400E-94AB-803E6E938533}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="19" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
+        <v>233</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I3" t="s">
+        <v>233</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J3" xr:uid="{FD737D12-8111-43F6-9CC8-0ED0805FC485}">
+      <formula1>"TRUE,FALSE,-"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF530C5-AF05-45C8-8B4A-B7812495957E}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="26" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2" xr:uid="{54717313-0510-4F30-AB6F-BB3447856BFA}">
+      <formula1>"TRUE,FALSE,-"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C37910F-4799-4014-9A7A-01BBA77DFC21}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="26" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2" xr:uid="{BC860AA8-DE2A-4F3C-BD78-6950880A9C34}">
+      <formula1>"TRUE,FALSE,-"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" location="LigtOp" xr:uid="{7549DFDC-3425-40E6-B896-A151AAE3186B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="700" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>158</v>
       </c>
@@ -1890,7 +2274,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1913,7 +2297,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -1936,7 +2320,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -1959,7 +2343,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -1979,7 +2363,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -1999,7 +2383,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -2019,7 +2403,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>194</v>
       </c>
@@ -2036,7 +2420,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2050,7 +2434,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>199</v>
       </c>
@@ -2058,7 +2442,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>201</v>
       </c>
@@ -2066,7 +2450,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>203</v>
       </c>
@@ -2074,7 +2458,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>205</v>
       </c>
@@ -2082,7 +2466,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>207</v>
       </c>
@@ -2090,7 +2474,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>209</v>
       </c>
@@ -2098,7 +2482,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>211</v>
       </c>
@@ -2106,42 +2490,42 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>218</v>
       </c>

</xml_diff>

<commit_message>
Added test and sorting of RelationChangeScreen.fill_existing_relations_list + namedTuple
</commit_message>
<xml_diff>
--- a/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template2.xlsx
+++ b/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\OTLMOW-GUI\demo_projects\simpel_vergelijkings_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5D258F-BB47-4738-B60B-E7E89163621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC73588D-A8EE-4905-913F-3D5C3F41F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="installatie#Verkeersbordopstell" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="242">
   <si>
     <t>typeURI</t>
   </si>
@@ -707,9 +707,6 @@
     <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Bevestiging</t>
   </si>
   <si>
-    <t>dummy_hXI</t>
-  </si>
-  <si>
     <t>dummy_zQp</t>
   </si>
   <si>
@@ -734,9 +731,6 @@
     <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#HoortBij</t>
   </si>
   <si>
-    <t>self_assigned</t>
-  </si>
-  <si>
     <t>dummy_LxexRM</t>
   </si>
   <si>
@@ -747,6 +741,18 @@
   </si>
   <si>
     <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#LigtOp</t>
+  </si>
+  <si>
+    <t>dummy_bevestiging_1</t>
+  </si>
+  <si>
+    <t>dummy_bevestiging_2</t>
+  </si>
+  <si>
+    <t>dummy_hoort_bij</t>
+  </si>
+  <si>
+    <t>dummy_ligt_op</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1336,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,7 +1718,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,7 +1951,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,10 +1998,10 @@
         <v>225</v>
       </c>
       <c r="B2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" t="s">
         <v>226</v>
-      </c>
-      <c r="C2" t="s">
-        <v>227</v>
       </c>
       <c r="D2" t="s">
         <v>95</v>
@@ -2004,7 +2010,7 @@
         <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G2" t="s">
         <v>61</v>
@@ -2013,7 +2019,7 @@
         <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J2" t="s">
         <v>29</v>
@@ -2024,28 +2030,28 @@
         <v>225</v>
       </c>
       <c r="B3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" t="s">
         <v>226</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>227</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>228</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>229</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>230</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>231</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>232</v>
-      </c>
-      <c r="I3" t="s">
-        <v>233</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
@@ -2065,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF530C5-AF05-45C8-8B4A-B7812495957E}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,13 +2114,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" t="s">
         <v>234</v>
-      </c>
-      <c r="B2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" t="s">
-        <v>236</v>
       </c>
       <c r="D2" t="s">
         <v>124</v>
@@ -2123,7 +2129,7 @@
         <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -2132,7 +2138,7 @@
         <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J2" t="s">
         <v>28</v>
@@ -2152,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C37910F-4799-4014-9A7A-01BBA77DFC21}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,13 +2201,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>61</v>
@@ -2210,7 +2216,7 @@
         <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G2" t="s">
         <v>61</v>
@@ -2219,7 +2225,7 @@
         <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added test for ExportDataDomain.generate_files for unedited excel files exported to an excel file
</commit_message>
<xml_diff>
--- a/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template2.xlsx
+++ b/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template2.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\OTLMOW-GUI\demo_projects\simpel_vergelijkings_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC73588D-A8EE-4905-913F-3D5C3F41F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411D0BFE-2591-44E0-B33C-0434E576222E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="installatie#Verkeersbordopstell" sheetId="1" r:id="rId1"/>
-    <sheet name="onderdeel#Funderingsmassief" sheetId="2" r:id="rId2"/>
-    <sheet name="onderdeel#Pictogram" sheetId="3" r:id="rId3"/>
-    <sheet name="onderdeel#Verkeersbordsteun" sheetId="4" r:id="rId4"/>
-    <sheet name="onderdeel#Bevestiging" sheetId="6" r:id="rId5"/>
-    <sheet name="onderdeel#HoortBij" sheetId="7" r:id="rId6"/>
-    <sheet name="onderdeel#LigtOp" sheetId="8" r:id="rId7"/>
+    <sheet name="ins#Verkeersbordopstelling" sheetId="1" r:id="rId1"/>
+    <sheet name="ond#Funderingsmassief" sheetId="2" r:id="rId2"/>
+    <sheet name="ond#Pictogram" sheetId="3" r:id="rId3"/>
+    <sheet name="ond#Verkeersbordsteun" sheetId="4" r:id="rId4"/>
+    <sheet name="ond#Bevestiging" sheetId="6" r:id="rId5"/>
+    <sheet name="ond#HoortBij" sheetId="7" r:id="rId6"/>
+    <sheet name="ond#LigtOp" sheetId="8" r:id="rId7"/>
     <sheet name="Keuzelijsten" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="242">
   <si>
     <t>typeURI</t>
   </si>
@@ -797,9 +797,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1106,7 +1107,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1337,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,12 +2160,12 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="20.7109375" customWidth="1"/>
+    <col min="1" max="25" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2227,16 +2228,11 @@
       <c r="I2" t="s">
         <v>236</v>
       </c>
-      <c r="J2" t="b">
-        <v>0</v>
+      <c r="J2" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="J2" xr:uid="{BC860AA8-DE2A-4F3C-BD78-6950880A9C34}">
-      <formula1>"TRUE,FALSE,-"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" location="LigtOp" xr:uid="{7549DFDC-3425-40E6-B896-A151AAE3186B}"/>
   </hyperlinks>

</xml_diff>